<commit_message>
updated code and analysis
</commit_message>
<xml_diff>
--- a/Analysis/Q1/Q1-OverallSimulationStats-Without.xlsx
+++ b/Analysis/Q1/Q1-OverallSimulationStats-Without.xlsx
@@ -1,39 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sal46633/Documents/GitHub/MobsSimulator-Python/Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sal46633/Documents/pythonEnvs/Google_Env/lib/python3.7/site-packages/MyPythonCode/Analysis/Q1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B70B742D-4185-3B4F-B0E8-9C9842C47C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2DD733-6068-B849-9EBA-2706F16D87C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19000"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q1-OverallSimulationStats-Witho" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Q1-OverallSimulationStats-Witho'!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Q1-OverallSimulationStats-Witho'!$A$2:$A$11</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Q1-OverallSimulationStats-Witho'!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Q1-OverallSimulationStats-Witho'!$B$2:$B$11</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Q1-OverallSimulationStats-Witho'!$C$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Q1-OverallSimulationStats-Witho'!$C$2:$C$11</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Q1-OverallSimulationStats-Witho'!$D$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Q1-OverallSimulationStats-Witho'!$D$2:$D$11</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">'Q1-OverallSimulationStats-Witho'!$B$1</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">'Q1-OverallSimulationStats-Witho'!$B$2:$B$11</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">'Q1-OverallSimulationStats-Witho'!$C$1</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">'Q1-OverallSimulationStats-Witho'!$C$2:$C$11</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">'Q1-OverallSimulationStats-Witho'!$D$1</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">'Q1-OverallSimulationStats-Witho'!$D$2:$D$11</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">'Q1-OverallSimulationStats-Witho'!$A$1</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">'Q1-OverallSimulationStats-Witho'!$A$2:$A$11</definedName>
-  </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -55,8 +37,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,21 +173,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -388,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -503,21 +470,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -563,11 +515,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -700,7 +649,363 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Q1-OverallSimulationStats-Witho'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q1-OverallSimulationStats-Witho'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E487-094B-BE70-282F45E86B8F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q1-OverallSimulationStats-Witho'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mobs Fail Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Q1-OverallSimulationStats-Witho'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q1-OverallSimulationStats-Witho'!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.07</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E487-094B-BE70-282F45E86B8F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q1-OverallSimulationStats-Witho'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Participation Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="50000"/>
@@ -783,39 +1088,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Q1-OverallSimulationStats-Witho'!$B$2:$B$11</c:f>
+              <c:f>'Q1-OverallSimulationStats-Witho'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>48.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>48.06</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>47.97</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96.97</c:v>
+                  <c:v>47.99</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.200000000000003</c:v>
+                  <c:v>48.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>48.03</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>47.99</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>47.98</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>48.05</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>47.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -823,369 +1128,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-25E7-1740-B89C-78E2AFAF3591}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Q1-OverallSimulationStats-Witho'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mobs Fail Rate</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Q1-OverallSimulationStats-Witho'!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Q1-OverallSimulationStats-Witho'!$C$2:$C$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.03</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>62.8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>99.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-25E7-1740-B89C-78E2AFAF3591}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Q1-OverallSimulationStats-Witho'!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Average Participation Rate</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="6"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Q1-OverallSimulationStats-Witho'!$A$2:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Q1-OverallSimulationStats-Witho'!$D$2:$D$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>47.94</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>48.03</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>48.01</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>48.02</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>48.03</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>47.93</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>47.99</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>48.01</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>48.02</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>48.06</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-25E7-1740-B89C-78E2AFAF3591}"/>
+              <c16:uniqueId val="{00000002-E487-094B-BE70-282F45E86B8F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1200,11 +1143,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1317002991"/>
-        <c:axId val="1317004639"/>
+        <c:axId val="2134387632"/>
+        <c:axId val="438614383"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1317002991"/>
+        <c:axId val="2134387632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1246,12 +1189,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1261,7 +1201,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1317004639"/>
+        <c:crossAx val="438614383"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1269,7 +1209,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1317004639"/>
+        <c:axId val="438614383"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1297,12 +1237,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1312,7 +1249,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1317002991"/>
+        <c:crossAx val="2134387632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1339,12 +1276,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1957,23 +1891,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>864694</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>112889</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>374650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>566244</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>4775</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{048943B2-2D0D-144D-8DF5-1A85AF665B8B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B7E3F5F-C40D-770E-B60E-71A21EB30289}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2290,173 +2224,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W15" sqref="V15:W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>100</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
-        <v>47.94</v>
+      <c r="D2">
+        <v>48.02</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>20</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>100</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
+        <v>48.06</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>99.99</v>
+      </c>
+      <c r="C4">
+        <v>0.01</v>
+      </c>
+      <c r="D4">
+        <v>47.97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>96.93</v>
+      </c>
+      <c r="C5">
+        <v>3.07</v>
+      </c>
+      <c r="D5">
+        <v>47.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>37.68</v>
+      </c>
+      <c r="C6">
+        <v>62.32</v>
+      </c>
+      <c r="D6">
+        <v>48.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>0.66</v>
+      </c>
+      <c r="C7">
+        <v>99.34</v>
+      </c>
+      <c r="D7">
         <v>48.03</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>30</v>
-      </c>
-      <c r="B4" s="1">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
         <v>100</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D8">
+        <v>47.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>80</v>
+      </c>
+      <c r="B9">
         <v>0</v>
       </c>
-      <c r="D4" s="1">
-        <v>48.01</v>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>47.98</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>40</v>
-      </c>
-      <c r="B5" s="1">
-        <v>96.97</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3.03</v>
-      </c>
-      <c r="D5" s="1">
-        <v>48.02</v>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>48.05</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>50</v>
-      </c>
-      <c r="B6" s="1">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="C6" s="1">
-        <v>62.8</v>
-      </c>
-      <c r="D6" s="1">
-        <v>48.03</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>60</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>99.5</v>
-      </c>
-      <c r="D7" s="1">
-        <v>47.93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>70</v>
-      </c>
-      <c r="B8" s="1">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11">
         <v>0</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C11">
         <v>100</v>
       </c>
-      <c r="D8" s="1">
-        <v>47.99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>80</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>100</v>
-      </c>
-      <c r="D9" s="1">
-        <v>48.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>90</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>100</v>
-      </c>
-      <c r="D10" s="1">
-        <v>48.02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>100</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>100</v>
-      </c>
-      <c r="D11" s="1">
-        <v>48.06</v>
+      <c r="D11">
+        <v>47.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated code and added data
</commit_message>
<xml_diff>
--- a/Analysis/Q1/Q1-OverallSimulationStats-Without.xlsx
+++ b/Analysis/Q1/Q1-OverallSimulationStats-Without.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sal46633/Documents/pythonEnvs/Google_Env/lib/python3.7/site-packages/MyPythonCode/Analysis/Q1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sal46633/Documents/GitHub/MobsSimulator-Python/Analysis/Q1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2DD733-6068-B849-9EBA-2706F16D87C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65AA778-C484-534A-8B4B-24E6CB445AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="36680" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q1-OverallSimulationStats-Witho" sheetId="1" r:id="rId1"/>
@@ -610,7 +610,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="76200" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -649,7 +649,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -788,7 +788,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="76200" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -827,7 +827,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
@@ -966,7 +966,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="76200" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -999,18 +999,15 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="t" anchorCtr="0">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1189,7 +1186,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -1237,7 +1234,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -1276,7 +1273,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="3600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1891,16 +1888,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>374650</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1929,9 +1926,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1969,7 +1966,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2075,7 +2072,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2217,7 +2214,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2227,8 +2224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W15" sqref="V15:W15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>